<commit_message>
add 'urls' syntax-coloring scheme
</commit_message>
<xml_diff>
--- a/Making Text Pretty - Syntax Coloring and Color Palettes/Color Palettes/MishMash-EPP-Worksheet.xlsx
+++ b/Making Text Pretty - Syntax Coloring and Color Palettes/Color Palettes/MishMash-EPP-Worksheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="385">
   <si>
     <t>Name in JGSoft Custom Syntax Coloring Scheme</t>
   </si>
@@ -1172,6 +1172,9 @@
   </si>
   <si>
     <t>`r`n within quotes</t>
+  </si>
+  <si>
+    <t>urls</t>
   </si>
 </sst>
 </file>
@@ -2342,7 +2345,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="231">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2963,6 +2966,75 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="14" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="23" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="24" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="25" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5621,13 +5693,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5637,10 +5709,11 @@
     <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="186"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="186"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="179" t="s">
         <v>306</v>
       </c>
@@ -5657,8 +5730,11 @@
       <c r="F1" s="178" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G1" s="178" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="140" t="s">
         <v>56</v>
       </c>
@@ -5671,8 +5747,9 @@
       <c r="D2" s="141"/>
       <c r="E2" s="141"/>
       <c r="F2" s="141"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G2" s="95"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="140" t="s">
         <v>57</v>
       </c>
@@ -5687,8 +5764,9 @@
       <c r="F3" s="142" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G3" s="231"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="140" t="s">
         <v>54</v>
       </c>
@@ -5705,8 +5783,9 @@
       <c r="F4" s="143" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G4" s="96"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="140" t="s">
         <v>55</v>
       </c>
@@ -5721,8 +5800,9 @@
       </c>
       <c r="E5" s="144"/>
       <c r="F5" s="144"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G5" s="97"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="140" t="s">
         <v>58</v>
       </c>
@@ -5735,8 +5815,9 @@
       <c r="D6" s="145"/>
       <c r="E6" s="145"/>
       <c r="F6" s="145"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G6" s="98"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="140" t="s">
         <v>59</v>
       </c>
@@ -5751,8 +5832,9 @@
       <c r="F7" s="146" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G7" s="99"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="140" t="s">
         <v>60</v>
       </c>
@@ -5765,8 +5847,9 @@
       <c r="D8" s="147"/>
       <c r="E8" s="147"/>
       <c r="F8" s="147"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G8" s="232"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="140" t="s">
         <v>61</v>
       </c>
@@ -5779,8 +5862,9 @@
       <c r="F9" s="148" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G9" s="233"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="140" t="s">
         <v>1</v>
       </c>
@@ -5795,8 +5879,9 @@
       <c r="F10" s="180" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G10" s="234"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="140" t="s">
         <v>62</v>
       </c>
@@ -5809,8 +5894,9 @@
       <c r="D11" s="150"/>
       <c r="E11" s="150"/>
       <c r="F11" s="150"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G11" s="235"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="140" t="s">
         <v>63</v>
       </c>
@@ -5827,8 +5913,9 @@
       <c r="F12" s="151" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G12" s="236"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="140" t="s">
         <v>64</v>
       </c>
@@ -5847,8 +5934,9 @@
       <c r="F13" s="152" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G13" s="103"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="140" t="s">
         <v>65</v>
       </c>
@@ -5861,8 +5949,9 @@
       <c r="D14" s="153"/>
       <c r="E14" s="153"/>
       <c r="F14" s="153"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G14" s="237"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="140" t="s">
         <v>66</v>
       </c>
@@ -5875,8 +5964,9 @@
       <c r="D15" s="154"/>
       <c r="E15" s="154"/>
       <c r="F15" s="154"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G15" s="105"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="140" t="s">
         <v>67</v>
       </c>
@@ -5893,8 +5983,9 @@
       <c r="F16" s="182" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G16" s="238"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="140" t="s">
         <v>45</v>
       </c>
@@ -5905,11 +5996,12 @@
       <c r="D17" s="189"/>
       <c r="E17" s="189"/>
       <c r="F17" s="189"/>
-      <c r="G17" s="188" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G17" s="189" t="s">
+        <v>384</v>
+      </c>
+      <c r="H17" s="188"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="140" t="s">
         <v>116</v>
       </c>
@@ -5924,8 +6016,9 @@
       </c>
       <c r="E18" s="156"/>
       <c r="F18" s="156"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G18" s="108"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="140" t="s">
         <v>68</v>
       </c>
@@ -5944,8 +6037,9 @@
       <c r="F19" s="157" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G19" s="136"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="140" t="s">
         <v>69</v>
       </c>
@@ -5964,8 +6058,9 @@
       <c r="F20" s="158" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G20" s="239"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="140" t="s">
         <v>51</v>
       </c>
@@ -5980,8 +6075,9 @@
         <v>322</v>
       </c>
       <c r="F21" s="159"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G21" s="111"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="140" t="s">
         <v>70</v>
       </c>
@@ -5994,9 +6090,10 @@
       <c r="D22" s="191"/>
       <c r="E22" s="191"/>
       <c r="F22" s="191"/>
-      <c r="G22" s="187"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G22" s="240"/>
+      <c r="H22" s="187"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="140" t="s">
         <v>15</v>
       </c>
@@ -6011,8 +6108,9 @@
       <c r="F23" s="160" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G23" s="112"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="140" t="s">
         <v>37</v>
       </c>
@@ -6023,11 +6121,12 @@
       <c r="D24" s="190"/>
       <c r="E24" s="190"/>
       <c r="F24" s="190"/>
-      <c r="G24" s="188" t="s">
+      <c r="G24" s="190"/>
+      <c r="H24" s="188" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="140" t="s">
         <v>34</v>
       </c>
@@ -6040,8 +6139,9 @@
       <c r="D25" s="161"/>
       <c r="E25" s="161"/>
       <c r="F25" s="161"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G25" s="113"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="140" t="s">
         <v>71</v>
       </c>
@@ -6052,11 +6152,12 @@
       <c r="D26" s="162"/>
       <c r="E26" s="162"/>
       <c r="F26" s="162"/>
-      <c r="G26" s="188" t="s">
+      <c r="G26" s="134"/>
+      <c r="H26" s="188" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="140" t="s">
         <v>72</v>
       </c>
@@ -6071,8 +6172,9 @@
       <c r="F27" s="163" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G27" s="241"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="140" t="s">
         <v>73</v>
       </c>
@@ -6087,8 +6189,9 @@
       <c r="F28" s="181" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G28" s="242"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="140" t="s">
         <v>74</v>
       </c>
@@ -6107,8 +6210,9 @@
       <c r="F29" s="165" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G29" s="115"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="140" t="s">
         <v>75</v>
       </c>
@@ -6125,8 +6229,9 @@
       <c r="F30" s="166" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G30" s="116"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="140" t="s">
         <v>76</v>
       </c>
@@ -6141,8 +6246,9 @@
       <c r="F31" s="167" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G31" s="243"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="140" t="s">
         <v>77</v>
       </c>
@@ -6155,8 +6261,9 @@
       <c r="F32" s="168" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G32" s="118"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="140" t="s">
         <v>78</v>
       </c>
@@ -6169,8 +6276,9 @@
       <c r="F33" s="169" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G33" s="244"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="140" t="s">
         <v>79</v>
       </c>
@@ -6183,8 +6291,9 @@
       <c r="F34" s="170" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G34" s="245"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="140" t="s">
         <v>80</v>
       </c>
@@ -6197,8 +6306,9 @@
       <c r="F35" s="171" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G35" s="246"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="140" t="s">
         <v>81</v>
       </c>
@@ -6211,8 +6321,9 @@
       <c r="F36" s="172" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G36" s="247"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="140" t="s">
         <v>82</v>
       </c>
@@ -6225,8 +6336,9 @@
       <c r="F37" s="173" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G37" s="248"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="140" t="s">
         <v>83</v>
       </c>
@@ -6239,8 +6351,9 @@
       <c r="F38" s="174" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G38" s="249"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="140" t="s">
         <v>84</v>
       </c>
@@ -6255,8 +6368,9 @@
       <c r="F39" s="175" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G39" s="250"/>
+    </row>
+    <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="140" t="s">
         <v>85</v>
       </c>
@@ -6267,11 +6381,12 @@
       <c r="D40" s="139"/>
       <c r="E40" s="139"/>
       <c r="F40" s="139"/>
-      <c r="G40" s="188" t="s">
+      <c r="G40" s="251"/>
+      <c r="H40" s="188" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="140" t="s">
         <v>86</v>
       </c>
@@ -6284,9 +6399,10 @@
       <c r="D41" s="176"/>
       <c r="E41" s="176"/>
       <c r="F41" s="176"/>
-      <c r="G41" s="187"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G41" s="252"/>
+      <c r="H41" s="187"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="140" t="s">
         <v>87</v>
       </c>
@@ -6301,8 +6417,9 @@
       <c r="F42" s="135" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G42" s="253"/>
+    </row>
+    <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="140" t="s">
         <v>88</v>
       </c>
@@ -6315,8 +6432,9 @@
       <c r="F43" s="135" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G43" s="253"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
         <v>376</v>
       </c>

</xml_diff>

<commit_message>
Complete MishMash for EPP8, edit Schemes
</commit_message>
<xml_diff>
--- a/Making Text Pretty - Syntax Coloring and Color Palettes/Color Palettes/MishMash-EPP-Worksheet.xlsx
+++ b/Making Text Pretty - Syntax Coloring and Color Palettes/Color Palettes/MishMash-EPP-Worksheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="440">
   <si>
     <t>Name in JGSoft Custom Syntax Coloring Scheme</t>
   </si>
@@ -1404,29 +1404,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>[EPP8]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Metatoken</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>[EPP8: Gone]</t>
     </r>
     <r>
@@ -1785,12 +1762,131 @@
       <t xml:space="preserve"> Indentation level 4</t>
     </r>
   </si>
+  <si>
+    <t>Default + underline dashed wide</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[EPP8]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Meta token</t>
+    </r>
+  </si>
+  <si>
+    <t>210, 142, 0</t>
+  </si>
+  <si>
+    <t>81, 81, 81 over 190, 145, 231</t>
+  </si>
+  <si>
+    <t>230, 219, 116 BOLD</t>
+  </si>
+  <si>
+    <t>230, 219, 116 underline dash narrow</t>
+  </si>
+  <si>
+    <t>Default (otherwise it makes it lined paper)</t>
+  </si>
+  <si>
+    <t>68, 113, 82</t>
+  </si>
+  <si>
+    <t>67, 105, 141</t>
+  </si>
+  <si>
+    <t>140, 140, 140</t>
+  </si>
+  <si>
+    <t>folded line</t>
+  </si>
+  <si>
+    <t>66, 66, 66</t>
+  </si>
+  <si>
+    <t>49, 51, 53</t>
+  </si>
+  <si>
+    <t>85, 85, 85</t>
+  </si>
+  <si>
+    <t>174, 138, 190</t>
+  </si>
+  <si>
+    <t>Control Character</t>
+  </si>
+  <si>
+    <t>181, 98, 119</t>
+  </si>
+  <si>
+    <t>181, 181, 181</t>
+  </si>
+  <si>
+    <t>33, 66, 131</t>
+  </si>
+  <si>
+    <t>191, 191, 191</t>
+  </si>
+  <si>
+    <t>highlighted replacement</t>
+  </si>
+  <si>
+    <t>Default, dashed wide</t>
+  </si>
+  <si>
+    <t>Default, dashed narrow</t>
+  </si>
+  <si>
+    <t>Default, dashed dots</t>
+  </si>
+  <si>
+    <t>Default, single</t>
+  </si>
+  <si>
+    <t>another link option</t>
+  </si>
+  <si>
+    <t>HIDDEN HIDDEN HIDDEN</t>
+  </si>
+  <si>
+    <t>non-underlined of url blue</t>
+  </si>
+  <si>
+    <t>another purple</t>
+  </si>
+  <si>
+    <t>a bold version of default</t>
+  </si>
+  <si>
+    <t>an italics version of default</t>
+  </si>
+  <si>
+    <t>Markdown bold</t>
+  </si>
+  <si>
+    <t>Markdown italics</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="104" x14ac:knownFonts="1">
+  <fonts count="113" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2582,8 +2678,75 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF8C8C8C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF555555"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFCBD1D1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFB5B5B5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFBFBFBF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF589DF6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF7F9F7F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFCBD1D1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="29">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2747,6 +2910,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF264F78"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF447152"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF43698D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF424242"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAE8ABE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB56277"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF214283"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2958,7 +3157,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3122,9 +3321,6 @@
     <xf numFmtId="0" fontId="43" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3491,105 +3687,6 @@
     </xf>
     <xf numFmtId="0" fontId="94" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="103" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3611,6 +3708,150 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -3621,16 +3862,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF002B36"/>
-      <color rgb="FF264F78"/>
-      <color rgb="FF8EC074"/>
-      <color rgb="FFFBBC42"/>
-      <color rgb="FFFB5842"/>
-      <color rgb="FF71ABC2"/>
-      <color rgb="FFE6DB13"/>
-      <color rgb="FF728B72"/>
-      <color rgb="FFD1C79E"/>
-      <color rgb="FFCD5C5C"/>
+      <color rgb="FFA9B7C6"/>
+      <color rgb="FF32593D"/>
+      <color rgb="FFBFBFBF"/>
+      <color rgb="FF214283"/>
+      <color rgb="FFB5B5B5"/>
+      <color rgb="FFB56277"/>
+      <color rgb="FF555555"/>
+      <color rgb="FFAE8ABE"/>
+      <color rgb="FF313335"/>
+      <color rgb="FF606366"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3646,44 +3887,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1440180</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>272480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>15992</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>196642</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8191500" y="17996600"/>
-          <a:ext cx="9373352" cy="396602"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
@@ -3705,7 +3908,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3714,6 +3917,94 @@
         <a:xfrm>
           <a:off x="20962620" y="2133600"/>
           <a:ext cx="6485714" cy="3780952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1394460</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>142380</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8145780" y="18006060"/>
+          <a:ext cx="10058400" cy="332880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>31632</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2125980</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>31582</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12573000" y="15934572"/>
+          <a:ext cx="1866900" cy="822910"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3990,8 +4281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D47" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4013,76 +4304,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="240" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="232"/>
-      <c r="C1" s="232"/>
-      <c r="D1" s="233"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="242"/>
       <c r="E1" s="35"/>
-      <c r="F1" s="201" t="s">
+      <c r="F1" s="210" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="202"/>
-      <c r="H1" s="202"/>
-      <c r="I1" s="202"/>
-      <c r="J1" s="203"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="212"/>
       <c r="K1" s="45"/>
-      <c r="L1" s="219" t="s">
+      <c r="L1" s="228" t="s">
         <v>229</v>
       </c>
-      <c r="M1" s="220"/>
-      <c r="N1" s="221"/>
+      <c r="M1" s="229"/>
+      <c r="N1" s="230"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="213"/>
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="214"/>
+      <c r="A2" s="222"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="223"/>
       <c r="E2" s="32"/>
-      <c r="F2" s="204" t="s">
+      <c r="F2" s="213" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="205"/>
-      <c r="H2" s="205"/>
-      <c r="I2" s="205"/>
-      <c r="J2" s="206"/>
+      <c r="G2" s="214"/>
+      <c r="H2" s="214"/>
+      <c r="I2" s="214"/>
+      <c r="J2" s="215"/>
       <c r="K2" s="45"/>
-      <c r="L2" s="222"/>
-      <c r="M2" s="223"/>
-      <c r="N2" s="224"/>
+      <c r="L2" s="231"/>
+      <c r="M2" s="232"/>
+      <c r="N2" s="233"/>
     </row>
     <row r="3" spans="1:15" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="215"/>
-      <c r="B3" s="215"/>
-      <c r="C3" s="215"/>
-      <c r="D3" s="216"/>
+      <c r="A3" s="224"/>
+      <c r="B3" s="224"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="225"/>
       <c r="E3" s="33"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="208"/>
-      <c r="H3" s="208"/>
-      <c r="I3" s="208"/>
-      <c r="J3" s="209"/>
+      <c r="F3" s="216"/>
+      <c r="G3" s="217"/>
+      <c r="H3" s="217"/>
+      <c r="I3" s="217"/>
+      <c r="J3" s="218"/>
       <c r="K3" s="45"/>
-      <c r="L3" s="222"/>
-      <c r="M3" s="223"/>
-      <c r="N3" s="224"/>
+      <c r="L3" s="231"/>
+      <c r="M3" s="232"/>
+      <c r="N3" s="233"/>
     </row>
     <row r="4" spans="1:15" s="3" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="217"/>
-      <c r="B4" s="217"/>
-      <c r="C4" s="217"/>
-      <c r="D4" s="218"/>
+      <c r="A4" s="226"/>
+      <c r="B4" s="226"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="227"/>
       <c r="E4" s="33"/>
-      <c r="F4" s="210"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-      <c r="I4" s="211"/>
-      <c r="J4" s="212"/>
+      <c r="F4" s="219"/>
+      <c r="G4" s="220"/>
+      <c r="H4" s="220"/>
+      <c r="I4" s="220"/>
+      <c r="J4" s="221"/>
       <c r="K4" s="45"/>
-      <c r="L4" s="225"/>
-      <c r="M4" s="226"/>
-      <c r="N4" s="227"/>
+      <c r="L4" s="234"/>
+      <c r="M4" s="235"/>
+      <c r="N4" s="236"/>
     </row>
     <row r="5" spans="1:15" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
@@ -4144,13 +4435,13 @@
       <c r="G6" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="92" t="s">
+      <c r="H6" s="91" t="s">
         <v>256</v>
       </c>
       <c r="I6" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="J6" s="237" t="s">
+      <c r="J6" s="203" t="s">
         <v>160</v>
       </c>
       <c r="K6" s="45"/>
@@ -4175,7 +4466,7 @@
       <c r="G7" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="173" t="s">
+      <c r="H7" s="172" t="s">
         <v>265</v>
       </c>
       <c r="I7" s="6" t="s">
@@ -4185,11 +4476,11 @@
         <v>376</v>
       </c>
       <c r="K7" s="45"/>
-      <c r="L7" s="228" t="s">
+      <c r="L7" s="237" t="s">
         <v>185</v>
       </c>
-      <c r="M7" s="229"/>
-      <c r="N7" s="230"/>
+      <c r="M7" s="238"/>
+      <c r="N7" s="239"/>
       <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -4212,7 +4503,7 @@
       <c r="G8" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H8" s="93" t="s">
+      <c r="H8" s="92" t="s">
         <v>259</v>
       </c>
       <c r="I8" s="6" t="s">
@@ -4250,7 +4541,7 @@
         <v>57</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="178" t="s">
+      <c r="H9" s="177" t="s">
         <v>262</v>
       </c>
       <c r="I9" s="6" t="s">
@@ -4290,7 +4581,7 @@
       <c r="G10" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H10" s="94" t="s">
+      <c r="H10" s="93" t="s">
         <v>263</v>
       </c>
       <c r="I10" s="6" t="s">
@@ -4330,7 +4621,7 @@
       <c r="G11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="95" t="s">
+      <c r="H11" s="94" t="s">
         <v>260</v>
       </c>
       <c r="I11" s="6" t="s">
@@ -4370,7 +4661,7 @@
       <c r="G12" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H12" s="96" t="s">
+      <c r="H12" s="95" t="s">
         <v>261</v>
       </c>
       <c r="I12" s="6" t="s">
@@ -4408,8 +4699,15 @@
         <v>380</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="4"/>
+      <c r="H13" s="250" t="s">
+        <v>256</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>160</v>
+      </c>
       <c r="K13" s="46"/>
       <c r="L13" s="56" t="s">
         <v>171</v>
@@ -4439,7 +4737,7 @@
         <v>381</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="234" t="s">
+      <c r="H14" s="200" t="s">
         <v>256</v>
       </c>
       <c r="I14" s="6" t="s">
@@ -4477,8 +4775,15 @@
         <v>382</v>
       </c>
       <c r="G15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="4"/>
+      <c r="H15" s="256" t="s">
+        <v>432</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>160</v>
+      </c>
       <c r="K15" s="46"/>
       <c r="L15" s="59" t="s">
         <v>176</v>
@@ -4508,8 +4813,15 @@
         <v>383</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="4"/>
+      <c r="H16" s="249">
+        <v>1</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>421</v>
+      </c>
       <c r="K16" s="46"/>
       <c r="L16" s="60" t="s">
         <v>178</v>
@@ -4541,7 +4853,7 @@
       <c r="G17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="97" t="s">
+      <c r="H17" s="96" t="s">
         <v>264</v>
       </c>
       <c r="I17" s="6" t="s">
@@ -4581,7 +4893,7 @@
       <c r="G18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="235" t="s">
+      <c r="H18" s="201" t="s">
         <v>266</v>
       </c>
       <c r="I18" s="6" t="s">
@@ -4619,7 +4931,7 @@
         <v>61</v>
       </c>
       <c r="G19" s="6"/>
-      <c r="H19" s="180" t="s">
+      <c r="H19" s="179" t="s">
         <v>267</v>
       </c>
       <c r="I19" s="6" t="s">
@@ -4657,8 +4969,15 @@
         <v>384</v>
       </c>
       <c r="G20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="4"/>
+      <c r="H20" s="254" t="s">
+        <v>434</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>160</v>
+      </c>
       <c r="K20" s="46"/>
       <c r="L20" s="64" t="s">
         <v>181</v>
@@ -4687,9 +5006,18 @@
       <c r="F21" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="4"/>
+      <c r="G21" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="H21" s="91" t="s">
+        <v>436</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>160</v>
+      </c>
       <c r="K21" s="46"/>
       <c r="L21" s="69" t="s">
         <v>181</v>
@@ -4721,7 +5049,7 @@
       <c r="G22" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="98" t="s">
+      <c r="H22" s="97" t="s">
         <v>149</v>
       </c>
       <c r="I22" s="6" t="s">
@@ -4761,7 +5089,7 @@
       <c r="G23" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="H23" s="182" t="s">
+      <c r="H23" s="181" t="s">
         <v>245</v>
       </c>
       <c r="I23" s="6" t="s">
@@ -4801,13 +5129,13 @@
       <c r="G24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="183" t="s">
+      <c r="H24" s="182" t="s">
         <v>300</v>
       </c>
       <c r="I24" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="J24" s="238" t="s">
+      <c r="J24" s="204" t="s">
         <v>160</v>
       </c>
       <c r="K24" s="46"/>
@@ -4841,7 +5169,7 @@
       <c r="G25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="99" t="s">
+      <c r="H25" s="98" t="s">
         <v>268</v>
       </c>
       <c r="I25" s="6" t="s">
@@ -4881,7 +5209,7 @@
       <c r="G26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="184" t="s">
+      <c r="H26" s="183" t="s">
         <v>196</v>
       </c>
       <c r="I26" s="6" t="s">
@@ -4915,7 +5243,7 @@
       <c r="G27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="100" t="s">
+      <c r="H27" s="99" t="s">
         <v>270</v>
       </c>
       <c r="I27" s="6" t="s">
@@ -4946,9 +5274,18 @@
       <c r="F28" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="G28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="4"/>
+      <c r="G28" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="H28" s="257" t="s">
+        <v>437</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>160</v>
+      </c>
       <c r="K28" s="46"/>
       <c r="L28" s="50"/>
       <c r="M28" s="6"/>
@@ -4961,7 +5298,7 @@
       <c r="B29" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="C29" s="91" t="s">
+      <c r="C29" s="90" t="s">
         <v>248</v>
       </c>
       <c r="D29" s="42" t="s">
@@ -4974,7 +5311,7 @@
       <c r="G29" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H29" s="101" t="s">
+      <c r="H29" s="100" t="s">
         <v>271</v>
       </c>
       <c r="I29" s="6" t="s">
@@ -5003,8 +5340,15 @@
         <v>387</v>
       </c>
       <c r="G30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="4"/>
+      <c r="H30" s="255" t="s">
+        <v>435</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>160</v>
+      </c>
       <c r="K30" s="46"/>
       <c r="L30" s="48" t="s">
         <v>168</v>
@@ -5026,7 +5370,7 @@
         <v>45</v>
       </c>
       <c r="G31" s="6"/>
-      <c r="H31" s="170" t="s">
+      <c r="H31" s="169" t="s">
         <v>368</v>
       </c>
       <c r="I31" s="6" t="s">
@@ -5052,7 +5396,7 @@
       <c r="G32" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H32" s="103" t="s">
+      <c r="H32" s="102" t="s">
         <v>272</v>
       </c>
       <c r="I32" s="6" t="s">
@@ -5078,7 +5422,7 @@
       <c r="G33" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H33" s="118" t="s">
+      <c r="H33" s="117" t="s">
         <v>299</v>
       </c>
       <c r="I33" s="6" t="s">
@@ -5110,7 +5454,7 @@
       <c r="G34" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="H34" s="186">
+      <c r="H34" s="185">
         <v>24648434354</v>
       </c>
       <c r="I34" s="6" t="s">
@@ -5120,7 +5464,7 @@
         <v>160</v>
       </c>
       <c r="K34" s="46"/>
-      <c r="L34" s="115" t="s">
+      <c r="L34" s="114" t="s">
         <v>289</v>
       </c>
       <c r="M34" s="6" t="s">
@@ -5140,7 +5484,7 @@
       <c r="G35" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H35" s="105">
+      <c r="H35" s="104">
         <v>2.4654234640000001</v>
       </c>
       <c r="I35" s="6" t="s">
@@ -5164,7 +5508,7 @@
         <v>70</v>
       </c>
       <c r="G36" s="6"/>
-      <c r="H36" s="187" t="s">
+      <c r="H36" s="186" t="s">
         <v>374</v>
       </c>
       <c r="I36" s="6" t="s">
@@ -5174,7 +5518,7 @@
         <v>160</v>
       </c>
       <c r="K36" s="46"/>
-      <c r="L36" s="172" t="s">
+      <c r="L36" s="171" t="s">
         <v>374</v>
       </c>
       <c r="M36" s="6" t="s">
@@ -5194,7 +5538,7 @@
       <c r="G37" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="H37" s="106" t="s">
+      <c r="H37" s="105" t="s">
         <v>255</v>
       </c>
       <c r="I37" s="6" t="s">
@@ -5226,13 +5570,13 @@
       <c r="G38" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="171" t="s">
+      <c r="H38" s="170" t="s">
         <v>291</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="J38" s="238" t="s">
+      <c r="J38" s="204" t="s">
         <v>160</v>
       </c>
       <c r="K38" s="46"/>
@@ -5258,7 +5602,7 @@
       <c r="G39" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H39" s="107" t="s">
+      <c r="H39" s="106" t="s">
         <v>307</v>
       </c>
       <c r="I39" s="6" t="s">
@@ -5268,7 +5612,7 @@
         <v>160</v>
       </c>
       <c r="K39" s="46"/>
-      <c r="L39" s="82" t="s">
+      <c r="L39" s="81" t="s">
         <v>225</v>
       </c>
       <c r="M39" s="42" t="s">
@@ -5290,7 +5634,7 @@
       <c r="G40" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H40" s="116" t="s">
+      <c r="H40" s="115" t="s">
         <v>297</v>
       </c>
       <c r="I40" s="6" t="s">
@@ -5300,7 +5644,7 @@
         <v>160</v>
       </c>
       <c r="K40" s="46"/>
-      <c r="L40" s="85" t="s">
+      <c r="L40" s="84" t="s">
         <v>228</v>
       </c>
       <c r="M40" s="42" t="s">
@@ -5320,7 +5664,7 @@
         <v>72</v>
       </c>
       <c r="G41" s="6"/>
-      <c r="H41" s="188" t="s">
+      <c r="H41" s="187" t="s">
         <v>288</v>
       </c>
       <c r="I41" s="6" t="s">
@@ -5330,7 +5674,7 @@
         <v>278</v>
       </c>
       <c r="K41" s="46"/>
-      <c r="L41" s="78" t="s">
+      <c r="L41" s="77" t="s">
         <v>231</v>
       </c>
       <c r="M41" s="42" t="s">
@@ -5350,7 +5694,7 @@
         <v>73</v>
       </c>
       <c r="G42" s="6"/>
-      <c r="H42" s="108" t="s">
+      <c r="H42" s="107" t="s">
         <v>197</v>
       </c>
       <c r="I42" s="6" t="s">
@@ -5360,7 +5704,7 @@
         <v>160</v>
       </c>
       <c r="K42" s="46"/>
-      <c r="L42" s="87" t="s">
+      <c r="L42" s="86" t="s">
         <v>231</v>
       </c>
       <c r="M42" s="6" t="s">
@@ -5382,7 +5726,7 @@
       <c r="G43" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="H43" s="109" t="s">
+      <c r="H43" s="108" t="s">
         <v>258</v>
       </c>
       <c r="I43" s="6" t="s">
@@ -5406,7 +5750,7 @@
         <v>75</v>
       </c>
       <c r="G44" s="6"/>
-      <c r="H44" s="110" t="s">
+      <c r="H44" s="109" t="s">
         <v>275</v>
       </c>
       <c r="I44" s="6" t="s">
@@ -5416,7 +5760,7 @@
         <v>156</v>
       </c>
       <c r="K44" s="46"/>
-      <c r="L44" s="113" t="s">
+      <c r="L44" s="112" t="s">
         <v>249</v>
       </c>
       <c r="M44" s="6" t="s">
@@ -5436,7 +5780,7 @@
         <v>76</v>
       </c>
       <c r="G45" s="6"/>
-      <c r="H45" s="111" t="s">
+      <c r="H45" s="110" t="s">
         <v>276</v>
       </c>
       <c r="I45" s="6" t="s">
@@ -5446,7 +5790,7 @@
         <v>209</v>
       </c>
       <c r="K45" s="46"/>
-      <c r="L45" s="117" t="s">
+      <c r="L45" s="116" t="s">
         <v>280</v>
       </c>
       <c r="M45" s="6" t="s">
@@ -5466,7 +5810,7 @@
         <v>77</v>
       </c>
       <c r="G46" s="6"/>
-      <c r="H46" s="112" t="s">
+      <c r="H46" s="111" t="s">
         <v>277</v>
       </c>
       <c r="I46" s="6" t="s">
@@ -5476,7 +5820,7 @@
         <v>232</v>
       </c>
       <c r="K46" s="46"/>
-      <c r="L46" s="104" t="s">
+      <c r="L46" s="103" t="s">
         <v>269</v>
       </c>
       <c r="M46" s="42" t="s">
@@ -5496,7 +5840,7 @@
         <v>78</v>
       </c>
       <c r="G47" s="6"/>
-      <c r="H47" s="191" t="s">
+      <c r="H47" s="190" t="s">
         <v>254</v>
       </c>
       <c r="I47" s="6" t="s">
@@ -5506,7 +5850,7 @@
         <v>200</v>
       </c>
       <c r="K47" s="46"/>
-      <c r="L47" s="119" t="s">
+      <c r="L47" s="118" t="s">
         <v>280</v>
       </c>
       <c r="M47" s="42" t="s">
@@ -5526,7 +5870,7 @@
         <v>79</v>
       </c>
       <c r="G48" s="6"/>
-      <c r="H48" s="192" t="s">
+      <c r="H48" s="191" t="s">
         <v>249</v>
       </c>
       <c r="I48" s="6" t="s">
@@ -5536,7 +5880,7 @@
         <v>238</v>
       </c>
       <c r="K48" s="46"/>
-      <c r="L48" s="114" t="s">
+      <c r="L48" s="113" t="s">
         <v>178</v>
       </c>
       <c r="M48" s="6" t="s">
@@ -5556,7 +5900,7 @@
         <v>80</v>
       </c>
       <c r="G49" s="6"/>
-      <c r="H49" s="193" t="s">
+      <c r="H49" s="192" t="s">
         <v>250</v>
       </c>
       <c r="I49" s="6" t="s">
@@ -5566,7 +5910,7 @@
         <v>240</v>
       </c>
       <c r="K49" s="46"/>
-      <c r="L49" s="102" t="s">
+      <c r="L49" s="101" t="s">
         <v>273</v>
       </c>
       <c r="M49" s="42" t="s">
@@ -5586,7 +5930,7 @@
         <v>81</v>
       </c>
       <c r="G50" s="6"/>
-      <c r="H50" s="194" t="s">
+      <c r="H50" s="193" t="s">
         <v>251</v>
       </c>
       <c r="I50" s="6" t="s">
@@ -5610,7 +5954,7 @@
         <v>82</v>
       </c>
       <c r="G51" s="6"/>
-      <c r="H51" s="195" t="s">
+      <c r="H51" s="194" t="s">
         <v>252</v>
       </c>
       <c r="I51" s="6" t="s">
@@ -5634,7 +5978,7 @@
         <v>83</v>
       </c>
       <c r="G52" s="6"/>
-      <c r="H52" s="196" t="s">
+      <c r="H52" s="195" t="s">
         <v>274</v>
       </c>
       <c r="I52" s="6" t="s">
@@ -5658,7 +6002,7 @@
         <v>84</v>
       </c>
       <c r="G53" s="6"/>
-      <c r="H53" s="197" t="s">
+      <c r="H53" s="196" t="s">
         <v>290</v>
       </c>
       <c r="I53" s="6" t="s">
@@ -5682,7 +6026,7 @@
         <v>85</v>
       </c>
       <c r="G54" s="6"/>
-      <c r="H54" s="198" t="s">
+      <c r="H54" s="197" t="s">
         <v>306</v>
       </c>
       <c r="I54" s="6" t="s">
@@ -5706,7 +6050,7 @@
         <v>86</v>
       </c>
       <c r="G55" s="6"/>
-      <c r="H55" s="199" t="s">
+      <c r="H55" s="198" t="s">
         <v>257</v>
       </c>
       <c r="I55" s="6" t="s">
@@ -5732,7 +6076,7 @@
       <c r="G56" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H56" s="200" t="s">
+      <c r="H56" s="199" t="s">
         <v>280</v>
       </c>
       <c r="I56" s="6" t="s">
@@ -5756,8 +6100,8 @@
         <v>88</v>
       </c>
       <c r="G57" s="7"/>
-      <c r="H57" s="236" t="s">
-        <v>292</v>
+      <c r="H57" s="202" t="s">
+        <v>433</v>
       </c>
       <c r="I57" s="7" t="s">
         <v>160</v>
@@ -5776,13 +6120,13 @@
       <c r="C58" s="28"/>
       <c r="D58" s="11"/>
       <c r="E58" s="34"/>
-      <c r="F58" s="175" t="s">
+      <c r="F58" s="174" t="s">
         <v>89</v>
       </c>
-      <c r="G58" s="176"/>
-      <c r="H58" s="176"/>
-      <c r="I58" s="176"/>
-      <c r="J58" s="177"/>
+      <c r="G58" s="175"/>
+      <c r="H58" s="175"/>
+      <c r="I58" s="175"/>
+      <c r="J58" s="176"/>
       <c r="K58" s="46"/>
       <c r="L58" s="50"/>
       <c r="M58" s="6"/>
@@ -5793,12 +6137,12 @@
       <c r="B59" s="11"/>
       <c r="C59" s="28"/>
       <c r="D59" s="11"/>
-      <c r="E59" s="239"/>
+      <c r="E59" s="205"/>
       <c r="F59" s="43" t="s">
         <v>90</v>
       </c>
       <c r="G59" s="43"/>
-      <c r="H59" s="88" t="s">
+      <c r="H59" s="87" t="s">
         <v>233</v>
       </c>
       <c r="I59" s="43" t="s">
@@ -5817,12 +6161,12 @@
       <c r="B60" s="11"/>
       <c r="C60" s="28"/>
       <c r="D60" s="11"/>
-      <c r="E60" s="239"/>
+      <c r="E60" s="205"/>
       <c r="F60" s="6" t="s">
         <v>91</v>
       </c>
       <c r="G60" s="6"/>
-      <c r="H60" s="84" t="s">
+      <c r="H60" s="83" t="s">
         <v>226</v>
       </c>
       <c r="I60" s="6" t="s">
@@ -5841,12 +6185,12 @@
       <c r="B61" s="11"/>
       <c r="C61" s="28"/>
       <c r="D61" s="11"/>
-      <c r="E61" s="239"/>
+      <c r="E61" s="205"/>
       <c r="F61" s="6" t="s">
         <v>92</v>
       </c>
       <c r="G61" s="6"/>
-      <c r="H61" s="81" t="s">
+      <c r="H61" s="80" t="s">
         <v>282</v>
       </c>
       <c r="I61" s="6" t="s">
@@ -5865,12 +6209,12 @@
       <c r="B62" s="11"/>
       <c r="C62" s="28"/>
       <c r="D62" s="11"/>
-      <c r="E62" s="239"/>
+      <c r="E62" s="205"/>
       <c r="F62" s="6" t="s">
         <v>93</v>
       </c>
       <c r="G62" s="6"/>
-      <c r="H62" s="81" t="s">
+      <c r="H62" s="80" t="s">
         <v>281</v>
       </c>
       <c r="I62" s="6" t="s">
@@ -5889,12 +6233,12 @@
       <c r="B63" s="11"/>
       <c r="C63" s="28"/>
       <c r="D63" s="11"/>
-      <c r="E63" s="239"/>
+      <c r="E63" s="205"/>
       <c r="F63" s="6" t="s">
         <v>94</v>
       </c>
       <c r="G63" s="6"/>
-      <c r="H63" s="81" t="s">
+      <c r="H63" s="80" t="s">
         <v>283</v>
       </c>
       <c r="I63" s="6" t="s">
@@ -5913,13 +6257,20 @@
       <c r="B64" s="11"/>
       <c r="C64" s="28"/>
       <c r="D64" s="11"/>
-      <c r="E64" s="239"/>
+      <c r="E64" s="205"/>
       <c r="F64" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G64" s="6"/>
-      <c r="I64" s="6"/>
-      <c r="J64" s="6"/>
+      <c r="H64" s="251" t="s">
+        <v>422</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>423</v>
+      </c>
       <c r="K64" s="46"/>
       <c r="L64" s="50"/>
       <c r="M64" s="6"/>
@@ -5930,13 +6281,20 @@
       <c r="B65" s="11"/>
       <c r="C65" s="28"/>
       <c r="D65" s="11"/>
-      <c r="E65" s="239"/>
+      <c r="E65" s="205"/>
       <c r="F65" s="6" t="s">
         <v>98</v>
       </c>
       <c r="G65" s="6"/>
-      <c r="I65" s="6"/>
-      <c r="J65" s="6"/>
+      <c r="H65" s="248">
+        <v>9564</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>419</v>
+      </c>
       <c r="K65" s="46"/>
       <c r="L65" s="50"/>
       <c r="M65" s="6"/>
@@ -5947,12 +6305,15 @@
       <c r="B66" s="11"/>
       <c r="C66" s="28"/>
       <c r="D66" s="11"/>
-      <c r="E66" s="239"/>
+      <c r="E66" s="205"/>
       <c r="F66" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G66" s="6"/>
-      <c r="I66" s="6"/>
+      <c r="H66" s="91"/>
+      <c r="I66" s="6" t="s">
+        <v>413</v>
+      </c>
       <c r="J66" s="6"/>
       <c r="K66" s="46"/>
       <c r="L66" s="50"/>
@@ -5964,12 +6325,12 @@
       <c r="B67" s="11"/>
       <c r="C67" s="28"/>
       <c r="D67" s="11"/>
-      <c r="E67" s="239"/>
+      <c r="E67" s="205"/>
       <c r="F67" s="6" t="s">
         <v>95</v>
       </c>
       <c r="G67" s="6"/>
-      <c r="H67" s="83" t="s">
+      <c r="H67" s="82" t="s">
         <v>223</v>
       </c>
       <c r="I67" s="6" t="s">
@@ -5988,12 +6349,12 @@
       <c r="B68" s="11"/>
       <c r="C68" s="28"/>
       <c r="D68" s="11"/>
-      <c r="E68" s="239"/>
+      <c r="E68" s="205"/>
       <c r="F68" s="6" t="s">
         <v>96</v>
       </c>
       <c r="G68" s="6"/>
-      <c r="H68" s="79" t="s">
+      <c r="H68" s="78" t="s">
         <v>227</v>
       </c>
       <c r="I68" s="6" t="s">
@@ -6012,12 +6373,12 @@
       <c r="B69" s="11"/>
       <c r="C69" s="28"/>
       <c r="D69" s="11"/>
-      <c r="E69" s="239"/>
+      <c r="E69" s="205"/>
       <c r="F69" s="6" t="s">
         <v>97</v>
       </c>
       <c r="G69" s="6"/>
-      <c r="H69" s="80" t="s">
+      <c r="H69" s="79" t="s">
         <v>218</v>
       </c>
       <c r="I69" s="6" t="s">
@@ -6036,7 +6397,7 @@
       <c r="B70" s="11"/>
       <c r="C70" s="28"/>
       <c r="D70" s="11"/>
-      <c r="E70" s="239"/>
+      <c r="E70" s="205"/>
       <c r="F70" s="6" t="s">
         <v>99</v>
       </c>
@@ -6060,16 +6421,16 @@
       <c r="B71" s="11"/>
       <c r="C71" s="28"/>
       <c r="D71" s="11"/>
-      <c r="E71" s="239"/>
+      <c r="E71" s="205"/>
       <c r="F71" s="6" t="s">
         <v>100</v>
       </c>
       <c r="G71" s="6"/>
-      <c r="H71" s="77" t="s">
+      <c r="H71" s="247" t="s">
         <v>208</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="J71" s="44" t="s">
         <v>213</v>
@@ -6084,13 +6445,20 @@
       <c r="B72" s="11"/>
       <c r="C72" s="28"/>
       <c r="D72" s="11"/>
-      <c r="E72" s="239"/>
+      <c r="E72" s="205"/>
       <c r="F72" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G72" s="6"/>
-      <c r="I72" s="6"/>
-      <c r="J72" s="6"/>
+      <c r="H72" s="246" t="s">
+        <v>417</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>416</v>
+      </c>
       <c r="K72" s="45"/>
       <c r="L72" s="50"/>
       <c r="M72" s="6"/>
@@ -6101,12 +6469,12 @@
       <c r="B73" s="11"/>
       <c r="C73" s="28"/>
       <c r="D73" s="11"/>
-      <c r="E73" s="239"/>
+      <c r="E73" s="205"/>
       <c r="F73" s="6" t="s">
         <v>101</v>
       </c>
       <c r="G73" s="6"/>
-      <c r="H73" s="81" t="s">
+      <c r="H73" s="80" t="s">
         <v>284</v>
       </c>
       <c r="I73" s="6" t="s">
@@ -6125,12 +6493,15 @@
       <c r="B74" s="11"/>
       <c r="C74" s="28"/>
       <c r="D74" s="11"/>
-      <c r="E74" s="239"/>
+      <c r="E74" s="205"/>
       <c r="F74" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G74" s="6"/>
-      <c r="I74" s="6"/>
+      <c r="H74" s="245"/>
+      <c r="I74" s="6" t="s">
+        <v>415</v>
+      </c>
       <c r="J74" s="6"/>
       <c r="K74" s="45"/>
       <c r="L74" s="50"/>
@@ -6142,12 +6513,15 @@
       <c r="B75" s="29"/>
       <c r="C75" s="30"/>
       <c r="D75" s="29"/>
-      <c r="E75" s="240"/>
+      <c r="E75" s="206"/>
       <c r="F75" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G75" s="6"/>
-      <c r="I75" s="6"/>
+      <c r="H75" s="244"/>
+      <c r="I75" s="6" t="s">
+        <v>414</v>
+      </c>
       <c r="J75" s="6"/>
       <c r="K75" s="45"/>
       <c r="L75" s="50"/>
@@ -6156,10 +6530,13 @@
     </row>
     <row r="76" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F76" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G76" s="6"/>
-      <c r="I76" s="6"/>
+      <c r="H76" s="91"/>
+      <c r="I76" s="6" t="s">
+        <v>428</v>
+      </c>
       <c r="J76" s="6"/>
       <c r="K76" s="45"/>
       <c r="L76" s="50"/>
@@ -6168,10 +6545,13 @@
     </row>
     <row r="77" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F77" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G77" s="6"/>
-      <c r="I77" s="6"/>
+      <c r="H77" s="91"/>
+      <c r="I77" s="6" t="s">
+        <v>429</v>
+      </c>
       <c r="J77" s="6"/>
       <c r="K77" s="45"/>
       <c r="L77" s="50"/>
@@ -6180,10 +6560,13 @@
     </row>
     <row r="78" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F78" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G78" s="6"/>
-      <c r="I78" s="6"/>
+      <c r="H78" s="91"/>
+      <c r="I78" s="6" t="s">
+        <v>430</v>
+      </c>
       <c r="J78" s="6"/>
       <c r="K78" s="45"/>
       <c r="L78" s="50"/>
@@ -6192,10 +6575,13 @@
     </row>
     <row r="79" spans="1:14" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F79" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G79" s="6"/>
-      <c r="I79" s="6"/>
+      <c r="H79" s="91"/>
+      <c r="I79" s="6" t="s">
+        <v>431</v>
+      </c>
       <c r="J79" s="6"/>
       <c r="K79" s="45"/>
       <c r="L79" s="50"/>
@@ -6207,7 +6593,7 @@
         <v>102</v>
       </c>
       <c r="G80" s="6"/>
-      <c r="H80" s="241" t="s">
+      <c r="H80" s="207" t="s">
         <v>215</v>
       </c>
       <c r="I80" s="6" t="s">
@@ -6215,6 +6601,15 @@
       </c>
       <c r="J80" s="37" t="s">
         <v>160</v>
+      </c>
+      <c r="L80" s="85" t="s">
+        <v>285</v>
+      </c>
+      <c r="M80" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="N80" s="6" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="81" spans="6:10" x14ac:dyDescent="0.3">
@@ -6222,30 +6617,37 @@
         <v>103</v>
       </c>
       <c r="G81" s="6"/>
-      <c r="H81" s="86" t="s">
+      <c r="H81" s="253" t="s">
         <v>285</v>
       </c>
       <c r="I81" s="6" t="s">
-        <v>144</v>
+        <v>426</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>230</v>
+        <v>425</v>
       </c>
     </row>
     <row r="82" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F82" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G82" s="6"/>
-      <c r="I82" s="6"/>
-      <c r="J82" s="6"/>
+      <c r="H82" s="252" t="s">
+        <v>427</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="J82" s="6" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="83" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F83" s="6" t="s">
         <v>104</v>
       </c>
       <c r="G83" s="6"/>
-      <c r="H83" s="90" t="s">
+      <c r="H83" s="89" t="s">
         <v>286</v>
       </c>
       <c r="I83" s="6" t="s">
@@ -6260,7 +6662,7 @@
         <v>105</v>
       </c>
       <c r="G84" s="7"/>
-      <c r="H84" s="89" t="s">
+      <c r="H84" s="88" t="s">
         <v>287</v>
       </c>
       <c r="I84" s="7" t="s">
@@ -6271,13 +6673,13 @@
       </c>
     </row>
     <row r="85" spans="6:10" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="F85" s="175" t="s">
+      <c r="F85" s="174" t="s">
         <v>106</v>
       </c>
-      <c r="G85" s="176"/>
-      <c r="H85" s="176"/>
-      <c r="I85" s="176"/>
-      <c r="J85" s="177"/>
+      <c r="G85" s="175"/>
+      <c r="H85" s="175"/>
+      <c r="I85" s="175"/>
+      <c r="J85" s="176"/>
     </row>
     <row r="86" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F86" s="43"/>
@@ -6286,7 +6688,7 @@
       <c r="I86" s="43"/>
       <c r="J86" s="43"/>
     </row>
-    <row r="87" spans="6:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="6:10" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
       <c r="H87" s="7"/>
@@ -6294,17 +6696,17 @@
       <c r="J87" s="7"/>
     </row>
     <row r="88" spans="6:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="F88" s="242" t="s">
+      <c r="F88" s="208" t="s">
         <v>388</v>
       </c>
       <c r="G88" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H88" s="174" t="s">
+      <c r="H88" s="173" t="s">
         <v>148</v>
       </c>
-      <c r="I88" s="174"/>
-      <c r="J88" s="174"/>
+      <c r="I88" s="173"/>
+      <c r="J88" s="173"/>
     </row>
     <row r="89" spans="6:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="F89" s="6" t="s">
@@ -6313,27 +6715,31 @@
       <c r="G89" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H89" s="174"/>
-      <c r="I89" s="174"/>
-      <c r="J89" s="174"/>
+      <c r="H89" s="173"/>
+      <c r="I89" s="173"/>
+      <c r="J89" s="173"/>
     </row>
     <row r="90" spans="6:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="F90" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="G90" s="6"/>
-      <c r="H90" s="174"/>
-      <c r="I90" s="174"/>
-      <c r="J90" s="174"/>
+      <c r="G90" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="H90" s="173"/>
+      <c r="I90" s="173"/>
+      <c r="J90" s="173"/>
     </row>
     <row r="91" spans="6:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="F91" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="G91" s="6"/>
-      <c r="H91" s="174"/>
-      <c r="I91" s="174"/>
-      <c r="J91" s="174"/>
+      <c r="G91" s="243" t="s">
+        <v>407</v>
+      </c>
+      <c r="H91" s="173"/>
+      <c r="I91" s="173"/>
+      <c r="J91" s="173"/>
     </row>
     <row r="92" spans="6:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="F92" s="6" t="s">
@@ -6342,76 +6748,86 @@
       <c r="G92" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="H92" s="174"/>
-      <c r="I92" s="174"/>
-      <c r="J92" s="174"/>
+      <c r="H92" s="173"/>
+      <c r="I92" s="173"/>
+      <c r="J92" s="173"/>
     </row>
     <row r="93" spans="6:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="F93" s="6" t="s">
-        <v>391</v>
-      </c>
-      <c r="G93" s="6"/>
-      <c r="H93" s="174"/>
-      <c r="I93" s="174"/>
-      <c r="J93" s="174"/>
+        <v>408</v>
+      </c>
+      <c r="G93" s="243" t="s">
+        <v>410</v>
+      </c>
+      <c r="H93" s="173"/>
+      <c r="I93" s="173"/>
+      <c r="J93" s="173"/>
     </row>
     <row r="94" spans="6:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="F94" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G94" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="H94" s="174"/>
-      <c r="I94" s="174"/>
-      <c r="J94" s="174"/>
+      <c r="H94" s="173"/>
+      <c r="I94" s="173"/>
+      <c r="J94" s="173"/>
     </row>
     <row r="95" spans="6:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="F95" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G95" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="H95" s="174"/>
-      <c r="I95" s="174"/>
-      <c r="J95" s="174"/>
+      <c r="H95" s="173"/>
+      <c r="I95" s="173"/>
+      <c r="J95" s="173"/>
     </row>
     <row r="96" spans="6:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="F96" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="G96" s="6"/>
-      <c r="H96" s="174"/>
-      <c r="I96" s="174"/>
-      <c r="J96" s="174"/>
+        <v>393</v>
+      </c>
+      <c r="G96" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="H96" s="173"/>
+      <c r="I96" s="173"/>
+      <c r="J96" s="173"/>
     </row>
     <row r="97" spans="6:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="F97" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="G97" s="6"/>
-      <c r="H97" s="174"/>
-      <c r="I97" s="174"/>
-      <c r="J97" s="174"/>
+        <v>394</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H97" s="173"/>
+      <c r="I97" s="173"/>
+      <c r="J97" s="173"/>
     </row>
     <row r="98" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F98" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H98" s="209"/>
+      <c r="I98" s="209"/>
+      <c r="J98" s="209"/>
+    </row>
+    <row r="99" spans="6:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F99" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G98" s="6"/>
-      <c r="H98" s="243"/>
-      <c r="I98" s="243"/>
-      <c r="J98" s="243"/>
-    </row>
-    <row r="99" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F99" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="G99" s="6"/>
-      <c r="H99" s="243"/>
-      <c r="I99" s="243"/>
-      <c r="J99" s="243"/>
+      <c r="G99" s="243" t="s">
+        <v>412</v>
+      </c>
+      <c r="H99" s="209"/>
+      <c r="I99" s="209"/>
+      <c r="J99" s="209"/>
     </row>
     <row r="100" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F100" s="6" t="s">
@@ -6420,9 +6836,9 @@
       <c r="G100" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="H100" s="243"/>
-      <c r="I100" s="243"/>
-      <c r="J100" s="243"/>
+      <c r="H100" s="209"/>
+      <c r="I100" s="209"/>
+      <c r="J100" s="209"/>
     </row>
     <row r="101" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F101" s="6" t="s">
@@ -6431,9 +6847,9 @@
       <c r="G101" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H101" s="243"/>
-      <c r="I101" s="243"/>
-      <c r="J101" s="243"/>
+      <c r="H101" s="209"/>
+      <c r="I101" s="209"/>
+      <c r="J101" s="209"/>
     </row>
     <row r="102" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F102" s="6" t="s">
@@ -6442,9 +6858,9 @@
       <c r="G102" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H102" s="243"/>
-      <c r="I102" s="243"/>
-      <c r="J102" s="243"/>
+      <c r="H102" s="209"/>
+      <c r="I102" s="209"/>
+      <c r="J102" s="209"/>
     </row>
     <row r="103" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F103" s="6" t="s">
@@ -6453,9 +6869,9 @@
       <c r="G103" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H103" s="243"/>
-      <c r="I103" s="243"/>
-      <c r="J103" s="243"/>
+      <c r="H103" s="209"/>
+      <c r="I103" s="209"/>
+      <c r="J103" s="209"/>
     </row>
     <row r="104" spans="6:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F104" s="7" t="s">
@@ -6464,9 +6880,9 @@
       <c r="G104" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H104" s="243"/>
-      <c r="I104" s="243"/>
-      <c r="J104" s="243"/>
+      <c r="H104" s="209"/>
+      <c r="I104" s="209"/>
+      <c r="J104" s="209"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -6502,731 +6918,731 @@
     <col min="4" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="167"/>
+    <col min="8" max="8" width="8.88671875" style="166"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="159" t="s">
         <v>301</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159" t="s">
+      <c r="B1" s="158"/>
+      <c r="C1" s="158" t="s">
         <v>302</v>
       </c>
-      <c r="D1" s="159" t="s">
+      <c r="D1" s="158" t="s">
         <v>310</v>
       </c>
-      <c r="E1" s="159" t="s">
+      <c r="E1" s="158" t="s">
         <v>303</v>
       </c>
-      <c r="F1" s="159" t="s">
+      <c r="F1" s="158" t="s">
         <v>304</v>
       </c>
-      <c r="G1" s="159" t="s">
+      <c r="G1" s="158" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="120" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="121" t="s">
         <v>259</v>
       </c>
-      <c r="C2" s="122" t="s">
+      <c r="C2" s="121" t="s">
         <v>354</v>
       </c>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="93"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="92"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="120" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="122" t="s">
         <v>262</v>
       </c>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123" t="s">
+      <c r="C3" s="122"/>
+      <c r="D3" s="122" t="s">
         <v>379</v>
       </c>
-      <c r="E3" s="123" t="s">
+      <c r="E3" s="122" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="123" t="s">
+      <c r="F3" s="122" t="s">
         <v>336</v>
       </c>
-      <c r="G3" s="178"/>
+      <c r="G3" s="177"/>
     </row>
     <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="123" t="s">
         <v>263</v>
       </c>
-      <c r="C4" s="164" t="s">
+      <c r="C4" s="163" t="s">
         <v>359</v>
       </c>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124" t="s">
+      <c r="D4" s="123"/>
+      <c r="E4" s="123" t="s">
         <v>321</v>
       </c>
-      <c r="F4" s="124" t="s">
+      <c r="F4" s="123" t="s">
         <v>334</v>
       </c>
-      <c r="G4" s="94"/>
+      <c r="G4" s="93"/>
     </row>
     <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="120" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="125" t="s">
+      <c r="B5" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="124" t="s">
         <v>352</v>
       </c>
-      <c r="D5" s="125" t="s">
+      <c r="D5" s="124" t="s">
         <v>309</v>
       </c>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="95"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="94"/>
     </row>
     <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="125" t="s">
         <v>261</v>
       </c>
-      <c r="C6" s="165" t="s">
+      <c r="C6" s="164" t="s">
         <v>362</v>
       </c>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="96"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="95"/>
     </row>
     <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="127" t="s">
+      <c r="B7" s="126" t="s">
         <v>264</v>
       </c>
-      <c r="C7" s="127" t="s">
+      <c r="C7" s="126" t="s">
         <v>355</v>
       </c>
-      <c r="D7" s="127"/>
-      <c r="E7" s="127"/>
-      <c r="F7" s="127" t="s">
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126" t="s">
         <v>335</v>
       </c>
-      <c r="G7" s="97"/>
+      <c r="G7" s="96"/>
     </row>
     <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="121" t="s">
+      <c r="A8" s="120" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="128" t="s">
+      <c r="B8" s="127" t="s">
         <v>266</v>
       </c>
-      <c r="C8" s="128" t="s">
+      <c r="C8" s="127" t="s">
         <v>356</v>
       </c>
-      <c r="D8" s="128"/>
-      <c r="E8" s="128"/>
-      <c r="F8" s="128"/>
-      <c r="G8" s="179"/>
+      <c r="D8" s="127"/>
+      <c r="E8" s="127"/>
+      <c r="F8" s="127"/>
+      <c r="G8" s="178"/>
     </row>
     <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="121" t="s">
+      <c r="A9" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="128" t="s">
         <v>267</v>
       </c>
-      <c r="C9" s="129"/>
-      <c r="D9" s="129"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129" t="s">
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128" t="s">
         <v>345</v>
       </c>
-      <c r="G9" s="180"/>
+      <c r="G9" s="179"/>
     </row>
     <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="130" t="s">
+      <c r="B10" s="129" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="130" t="s">
+      <c r="C10" s="129" t="s">
         <v>166</v>
       </c>
-      <c r="D10" s="130"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="161" t="s">
+      <c r="D10" s="129"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="160" t="s">
         <v>342</v>
       </c>
-      <c r="G10" s="181"/>
+      <c r="G10" s="180"/>
     </row>
     <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="120" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="131" t="s">
+      <c r="B11" s="130" t="s">
         <v>245</v>
       </c>
-      <c r="C11" s="131" t="s">
+      <c r="C11" s="130" t="s">
         <v>305</v>
       </c>
-      <c r="D11" s="131"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="182"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="181"/>
     </row>
     <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="132" t="s">
+      <c r="B12" s="131" t="s">
         <v>300</v>
       </c>
-      <c r="C12" s="132" t="s">
+      <c r="C12" s="131" t="s">
         <v>350</v>
       </c>
-      <c r="D12" s="132" t="s">
+      <c r="D12" s="131" t="s">
         <v>311</v>
       </c>
-      <c r="E12" s="132"/>
-      <c r="F12" s="132" t="s">
+      <c r="E12" s="131"/>
+      <c r="F12" s="131" t="s">
         <v>332</v>
       </c>
-      <c r="G12" s="183"/>
+      <c r="G12" s="182"/>
     </row>
     <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="121" t="s">
+      <c r="A13" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="133" t="s">
+      <c r="B13" s="132" t="s">
         <v>268</v>
       </c>
-      <c r="C13" s="133" t="s">
+      <c r="C13" s="132" t="s">
         <v>358</v>
       </c>
-      <c r="D13" s="133" t="s">
+      <c r="D13" s="132" t="s">
         <v>373</v>
       </c>
-      <c r="E13" s="133" t="s">
+      <c r="E13" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="133" t="s">
+      <c r="F13" s="132" t="s">
         <v>346</v>
       </c>
-      <c r="G13" s="99"/>
+      <c r="G13" s="98"/>
     </row>
     <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="134" t="s">
+      <c r="B14" s="133" t="s">
         <v>196</v>
       </c>
-      <c r="C14" s="134" t="s">
+      <c r="C14" s="133" t="s">
         <v>357</v>
       </c>
-      <c r="D14" s="134"/>
-      <c r="E14" s="134"/>
-      <c r="F14" s="134"/>
-      <c r="G14" s="184"/>
+      <c r="D14" s="133"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="183"/>
     </row>
     <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="121" t="s">
+      <c r="A15" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="135" t="s">
+      <c r="B15" s="134" t="s">
         <v>270</v>
       </c>
-      <c r="C15" s="135" t="s">
+      <c r="C15" s="134" t="s">
         <v>353</v>
       </c>
-      <c r="D15" s="135"/>
-      <c r="E15" s="135"/>
-      <c r="F15" s="135"/>
-      <c r="G15" s="100"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="134"/>
+      <c r="F15" s="134"/>
+      <c r="G15" s="99"/>
     </row>
     <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="121" t="s">
+      <c r="A16" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="136" t="s">
+      <c r="B16" s="135" t="s">
         <v>271</v>
       </c>
-      <c r="C16" s="136" t="s">
+      <c r="C16" s="135" t="s">
         <v>351</v>
       </c>
-      <c r="D16" s="136"/>
-      <c r="E16" s="136" t="s">
+      <c r="D16" s="135"/>
+      <c r="E16" s="135" t="s">
         <v>315</v>
       </c>
-      <c r="F16" s="163" t="s">
+      <c r="F16" s="162" t="s">
         <v>341</v>
       </c>
-      <c r="G16" s="185"/>
+      <c r="G16" s="184"/>
     </row>
     <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="121" t="s">
+      <c r="A17" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="170" t="s">
+      <c r="B17" s="169" t="s">
         <v>369</v>
       </c>
-      <c r="C17" s="170"/>
-      <c r="D17" s="170"/>
-      <c r="E17" s="170"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="170" t="s">
+      <c r="C17" s="169"/>
+      <c r="D17" s="169"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169" t="s">
         <v>379</v>
       </c>
-      <c r="H17" s="169"/>
+      <c r="H17" s="168"/>
     </row>
     <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="121" t="s">
+      <c r="A18" s="120" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="137" t="s">
+      <c r="B18" s="136" t="s">
         <v>272</v>
       </c>
-      <c r="C18" s="137" t="s">
+      <c r="C18" s="136" t="s">
         <v>364</v>
       </c>
-      <c r="D18" s="137" t="s">
+      <c r="D18" s="136" t="s">
         <v>311</v>
       </c>
-      <c r="E18" s="137"/>
-      <c r="F18" s="137"/>
-      <c r="G18" s="103"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="136"/>
+      <c r="G18" s="102"/>
     </row>
     <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="121" t="s">
+      <c r="A19" s="120" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="138" t="s">
+      <c r="B19" s="137" t="s">
         <v>299</v>
       </c>
-      <c r="C19" s="166" t="s">
+      <c r="C19" s="165" t="s">
         <v>363</v>
       </c>
-      <c r="D19" s="138" t="s">
+      <c r="D19" s="137" t="s">
         <v>324</v>
       </c>
-      <c r="E19" s="138" t="s">
+      <c r="E19" s="137" t="s">
         <v>323</v>
       </c>
-      <c r="F19" s="138" t="s">
+      <c r="F19" s="137" t="s">
         <v>338</v>
       </c>
-      <c r="G19" s="118"/>
+      <c r="G19" s="117"/>
     </row>
     <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="121" t="s">
+      <c r="A20" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="139">
+      <c r="B20" s="138">
         <v>24648434354</v>
       </c>
-      <c r="C20" s="139" t="s">
+      <c r="C20" s="138" t="s">
         <v>365</v>
       </c>
-      <c r="D20" s="139" t="s">
+      <c r="D20" s="138" t="s">
         <v>312</v>
       </c>
-      <c r="E20" s="139" t="s">
+      <c r="E20" s="138" t="s">
         <v>316</v>
       </c>
-      <c r="F20" s="139" t="s">
+      <c r="F20" s="138" t="s">
         <v>343</v>
       </c>
-      <c r="G20" s="186"/>
+      <c r="G20" s="185"/>
     </row>
     <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="121" t="s">
+      <c r="A21" s="120" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="140">
+      <c r="B21" s="139">
         <v>2.4654234640000001</v>
       </c>
-      <c r="C21" s="140" t="s">
+      <c r="C21" s="139" t="s">
         <v>317</v>
       </c>
-      <c r="D21" s="140"/>
-      <c r="E21" s="140" t="s">
+      <c r="D21" s="139"/>
+      <c r="E21" s="139" t="s">
         <v>317</v>
       </c>
-      <c r="F21" s="140"/>
-      <c r="G21" s="105"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="104"/>
     </row>
     <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="121" t="s">
+      <c r="A22" s="120" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="172" t="s">
+      <c r="B22" s="171" t="s">
         <v>374</v>
       </c>
-      <c r="C22" s="172" t="s">
+      <c r="C22" s="171" t="s">
         <v>378</v>
       </c>
-      <c r="D22" s="172"/>
-      <c r="E22" s="172"/>
-      <c r="F22" s="172"/>
-      <c r="G22" s="187"/>
-      <c r="H22" s="168"/>
+      <c r="D22" s="171"/>
+      <c r="E22" s="171"/>
+      <c r="F22" s="171"/>
+      <c r="G22" s="186"/>
+      <c r="H22" s="167"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="141" t="s">
+      <c r="B23" s="140" t="s">
         <v>255</v>
       </c>
-      <c r="C23" s="141" t="s">
+      <c r="C23" s="140" t="s">
         <v>360</v>
       </c>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141" t="s">
+      <c r="D23" s="140"/>
+      <c r="E23" s="140"/>
+      <c r="F23" s="140" t="s">
         <v>347</v>
       </c>
-      <c r="G23" s="106"/>
+      <c r="G23" s="105"/>
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="121" t="s">
+      <c r="A24" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="171" t="s">
+      <c r="B24" s="170" t="s">
         <v>291</v>
       </c>
-      <c r="C24" s="171"/>
-      <c r="D24" s="171"/>
-      <c r="E24" s="171"/>
-      <c r="F24" s="171"/>
-      <c r="G24" s="171"/>
-      <c r="H24" s="169" t="s">
+      <c r="C24" s="170"/>
+      <c r="D24" s="170"/>
+      <c r="E24" s="170"/>
+      <c r="F24" s="170"/>
+      <c r="G24" s="170"/>
+      <c r="H24" s="168" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="121" t="s">
+      <c r="A25" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="142" t="s">
+      <c r="B25" s="141" t="s">
         <v>202</v>
       </c>
-      <c r="C25" s="142" t="s">
+      <c r="C25" s="141" t="s">
         <v>361</v>
       </c>
-      <c r="D25" s="142"/>
-      <c r="E25" s="142"/>
-      <c r="F25" s="142"/>
-      <c r="G25" s="107"/>
+      <c r="D25" s="141"/>
+      <c r="E25" s="141"/>
+      <c r="F25" s="141"/>
+      <c r="G25" s="106"/>
     </row>
     <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="121" t="s">
+      <c r="A26" s="120" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="143" t="s">
+      <c r="B26" s="142" t="s">
         <v>297</v>
       </c>
-      <c r="C26" s="143"/>
-      <c r="D26" s="143"/>
-      <c r="E26" s="143"/>
-      <c r="F26" s="143"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="169" t="s">
+      <c r="C26" s="142"/>
+      <c r="D26" s="142"/>
+      <c r="E26" s="142"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="115"/>
+      <c r="H26" s="168" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="121" t="s">
+      <c r="A27" s="120" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="144" t="s">
+      <c r="B27" s="143" t="s">
         <v>288</v>
       </c>
-      <c r="C27" s="144"/>
-      <c r="D27" s="144"/>
-      <c r="E27" s="144" t="s">
+      <c r="C27" s="143"/>
+      <c r="D27" s="143"/>
+      <c r="E27" s="143" t="s">
         <v>313</v>
       </c>
-      <c r="F27" s="144" t="s">
+      <c r="F27" s="143" t="s">
         <v>344</v>
       </c>
-      <c r="G27" s="188"/>
+      <c r="G27" s="187"/>
     </row>
     <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="121" t="s">
+      <c r="A28" s="120" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="145" t="s">
+      <c r="B28" s="144" t="s">
         <v>197</v>
       </c>
-      <c r="C28" s="145"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145" t="s">
+      <c r="C28" s="144"/>
+      <c r="D28" s="144"/>
+      <c r="E28" s="144" t="s">
         <v>319</v>
       </c>
-      <c r="F28" s="162" t="s">
+      <c r="F28" s="161" t="s">
         <v>337</v>
       </c>
-      <c r="G28" s="189"/>
+      <c r="G28" s="188"/>
     </row>
     <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="121" t="s">
+      <c r="A29" s="120" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="146" t="s">
+      <c r="B29" s="145" t="s">
         <v>258</v>
       </c>
-      <c r="C29" s="146" t="s">
+      <c r="C29" s="145" t="s">
         <v>349</v>
       </c>
-      <c r="D29" s="146"/>
-      <c r="E29" s="146" t="s">
+      <c r="D29" s="145"/>
+      <c r="E29" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="146" t="s">
+      <c r="F29" s="145" t="s">
         <v>340</v>
       </c>
-      <c r="G29" s="109"/>
+      <c r="G29" s="108"/>
     </row>
     <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="121" t="s">
+      <c r="A30" s="120" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="147" t="s">
+      <c r="B30" s="146" t="s">
         <v>275</v>
       </c>
-      <c r="C30" s="147" t="s">
+      <c r="C30" s="146" t="s">
         <v>308</v>
       </c>
-      <c r="D30" s="147" t="s">
+      <c r="D30" s="146" t="s">
         <v>308</v>
       </c>
-      <c r="E30" s="147"/>
-      <c r="F30" s="147" t="s">
+      <c r="E30" s="146"/>
+      <c r="F30" s="146" t="s">
         <v>308</v>
       </c>
-      <c r="G30" s="110"/>
+      <c r="G30" s="109"/>
     </row>
     <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="121" t="s">
+      <c r="A31" s="120" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="148" t="s">
+      <c r="B31" s="147" t="s">
         <v>276</v>
       </c>
-      <c r="C31" s="148"/>
-      <c r="D31" s="148"/>
-      <c r="E31" s="148" t="s">
+      <c r="C31" s="147"/>
+      <c r="D31" s="147"/>
+      <c r="E31" s="147" t="s">
         <v>314</v>
       </c>
-      <c r="F31" s="148" t="s">
+      <c r="F31" s="147" t="s">
         <v>339</v>
       </c>
-      <c r="G31" s="190"/>
+      <c r="G31" s="189"/>
     </row>
     <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="121" t="s">
+      <c r="A32" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="149" t="s">
+      <c r="B32" s="148" t="s">
         <v>277</v>
       </c>
-      <c r="C32" s="149"/>
-      <c r="D32" s="149"/>
-      <c r="E32" s="149"/>
-      <c r="F32" s="149" t="s">
+      <c r="C32" s="148"/>
+      <c r="D32" s="148"/>
+      <c r="E32" s="148"/>
+      <c r="F32" s="148" t="s">
         <v>330</v>
       </c>
-      <c r="G32" s="112"/>
+      <c r="G32" s="111"/>
     </row>
     <row r="33" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="121" t="s">
+      <c r="A33" s="120" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="150" t="s">
+      <c r="B33" s="149" t="s">
         <v>254</v>
       </c>
-      <c r="C33" s="150"/>
-      <c r="D33" s="150"/>
-      <c r="E33" s="150"/>
-      <c r="F33" s="150" t="s">
+      <c r="C33" s="149"/>
+      <c r="D33" s="149"/>
+      <c r="E33" s="149"/>
+      <c r="F33" s="149" t="s">
         <v>333</v>
       </c>
-      <c r="G33" s="191"/>
+      <c r="G33" s="190"/>
     </row>
     <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="121" t="s">
+      <c r="A34" s="120" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="151" t="s">
+      <c r="B34" s="150" t="s">
         <v>249</v>
       </c>
-      <c r="C34" s="151"/>
-      <c r="D34" s="151"/>
-      <c r="E34" s="151"/>
-      <c r="F34" s="151" t="s">
+      <c r="C34" s="150"/>
+      <c r="D34" s="150"/>
+      <c r="E34" s="150"/>
+      <c r="F34" s="150" t="s">
         <v>325</v>
       </c>
-      <c r="G34" s="192"/>
+      <c r="G34" s="191"/>
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="121" t="s">
+      <c r="A35" s="120" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="152" t="s">
+      <c r="B35" s="151" t="s">
         <v>250</v>
       </c>
-      <c r="C35" s="152"/>
-      <c r="D35" s="152"/>
-      <c r="E35" s="152"/>
-      <c r="F35" s="152" t="s">
+      <c r="C35" s="151"/>
+      <c r="D35" s="151"/>
+      <c r="E35" s="151"/>
+      <c r="F35" s="151" t="s">
         <v>326</v>
       </c>
-      <c r="G35" s="193"/>
+      <c r="G35" s="192"/>
     </row>
     <row r="36" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="121" t="s">
+      <c r="A36" s="120" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="153" t="s">
+      <c r="B36" s="152" t="s">
         <v>251</v>
       </c>
-      <c r="C36" s="153"/>
-      <c r="D36" s="153"/>
-      <c r="E36" s="153"/>
-      <c r="F36" s="153" t="s">
+      <c r="C36" s="152"/>
+      <c r="D36" s="152"/>
+      <c r="E36" s="152"/>
+      <c r="F36" s="152" t="s">
         <v>327</v>
       </c>
-      <c r="G36" s="194"/>
+      <c r="G36" s="193"/>
     </row>
     <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="121" t="s">
+      <c r="A37" s="120" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="154" t="s">
+      <c r="B37" s="153" t="s">
         <v>252</v>
       </c>
-      <c r="C37" s="154"/>
-      <c r="D37" s="154"/>
-      <c r="E37" s="154"/>
-      <c r="F37" s="154" t="s">
+      <c r="C37" s="153"/>
+      <c r="D37" s="153"/>
+      <c r="E37" s="153"/>
+      <c r="F37" s="153" t="s">
         <v>328</v>
       </c>
-      <c r="G37" s="195"/>
+      <c r="G37" s="194"/>
     </row>
     <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="121" t="s">
+      <c r="A38" s="120" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="155" t="s">
+      <c r="B38" s="154" t="s">
         <v>274</v>
       </c>
-      <c r="C38" s="155"/>
-      <c r="D38" s="155"/>
-      <c r="E38" s="155"/>
-      <c r="F38" s="155" t="s">
+      <c r="C38" s="154"/>
+      <c r="D38" s="154"/>
+      <c r="E38" s="154"/>
+      <c r="F38" s="154" t="s">
         <v>329</v>
       </c>
-      <c r="G38" s="196"/>
+      <c r="G38" s="195"/>
     </row>
     <row r="39" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="121" t="s">
+      <c r="A39" s="120" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="156" t="s">
+      <c r="B39" s="155" t="s">
         <v>290</v>
       </c>
-      <c r="C39" s="156"/>
-      <c r="D39" s="156" t="s">
+      <c r="C39" s="155"/>
+      <c r="D39" s="155" t="s">
         <v>320</v>
       </c>
-      <c r="E39" s="156"/>
-      <c r="F39" s="156" t="s">
+      <c r="E39" s="155"/>
+      <c r="F39" s="155" t="s">
         <v>331</v>
       </c>
-      <c r="G39" s="197"/>
+      <c r="G39" s="196"/>
     </row>
     <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="121" t="s">
+      <c r="A40" s="120" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="120" t="s">
+      <c r="B40" s="119" t="s">
         <v>306</v>
       </c>
-      <c r="C40" s="120"/>
-      <c r="D40" s="120"/>
-      <c r="E40" s="120"/>
-      <c r="F40" s="120"/>
-      <c r="G40" s="198"/>
-      <c r="H40" s="169" t="s">
+      <c r="C40" s="119"/>
+      <c r="D40" s="119"/>
+      <c r="E40" s="119"/>
+      <c r="F40" s="119"/>
+      <c r="G40" s="197"/>
+      <c r="H40" s="168" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="121" t="s">
+      <c r="A41" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="157" t="s">
+      <c r="B41" s="156" t="s">
         <v>257</v>
       </c>
-      <c r="C41" s="157" t="s">
+      <c r="C41" s="156" t="s">
         <v>377</v>
       </c>
-      <c r="D41" s="157"/>
-      <c r="E41" s="157"/>
-      <c r="F41" s="157"/>
-      <c r="G41" s="199"/>
-      <c r="H41" s="168"/>
+      <c r="D41" s="156"/>
+      <c r="E41" s="156"/>
+      <c r="F41" s="156"/>
+      <c r="G41" s="198"/>
+      <c r="H41" s="167"/>
     </row>
     <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="121" t="s">
+      <c r="A42" s="120" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="117" t="s">
+      <c r="B42" s="116" t="s">
         <v>280</v>
       </c>
-      <c r="C42" s="117"/>
-      <c r="D42" s="117" t="s">
+      <c r="C42" s="116"/>
+      <c r="D42" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="E42" s="117" t="s">
+      <c r="E42" s="116" t="s">
         <v>322</v>
       </c>
-      <c r="F42" s="117" t="s">
+      <c r="F42" s="116" t="s">
         <v>348</v>
       </c>
-      <c r="G42" s="200"/>
+      <c r="G42" s="199"/>
     </row>
     <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="121" t="s">
+      <c r="A43" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="158" t="s">
+      <c r="B43" s="157" t="s">
         <v>292</v>
       </c>
-      <c r="C43" s="158"/>
-      <c r="D43" s="158"/>
-      <c r="E43" s="158"/>
-      <c r="F43" s="117" t="s">
+      <c r="C43" s="157"/>
+      <c r="D43" s="157"/>
+      <c r="E43" s="157"/>
+      <c r="F43" s="116" t="s">
         <v>370</v>
       </c>
-      <c r="G43" s="200"/>
+      <c r="G43" s="199"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F44" t="s">

</xml_diff>

<commit_message>
Update folding thickness and color
</commit_message>
<xml_diff>
--- a/Making Text Pretty - Syntax Coloring and Color Palettes/Color Palettes/MishMash-EPP-Worksheet.xlsx
+++ b/Making Text Pretty - Syntax Coloring and Color Palettes/Color Palettes/MishMash-EPP-Worksheet.xlsx
@@ -3708,6 +3708,48 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3807,50 +3849,8 @@
     <xf numFmtId="0" fontId="24" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="104" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="105" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="106" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="107" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="108" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="109" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="110" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="111" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="112" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4281,8 +4281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="D55" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4304,76 +4304,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="240" t="s">
+      <c r="A1" s="254" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="242"/>
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="256"/>
       <c r="E1" s="35"/>
-      <c r="F1" s="210" t="s">
+      <c r="F1" s="224" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="211"/>
-      <c r="H1" s="211"/>
-      <c r="I1" s="211"/>
-      <c r="J1" s="212"/>
+      <c r="G1" s="225"/>
+      <c r="H1" s="225"/>
+      <c r="I1" s="225"/>
+      <c r="J1" s="226"/>
       <c r="K1" s="45"/>
-      <c r="L1" s="228" t="s">
+      <c r="L1" s="242" t="s">
         <v>229</v>
       </c>
-      <c r="M1" s="229"/>
-      <c r="N1" s="230"/>
+      <c r="M1" s="243"/>
+      <c r="N1" s="244"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="222"/>
-      <c r="B2" s="222"/>
-      <c r="C2" s="222"/>
-      <c r="D2" s="223"/>
+      <c r="A2" s="236"/>
+      <c r="B2" s="236"/>
+      <c r="C2" s="236"/>
+      <c r="D2" s="237"/>
       <c r="E2" s="32"/>
-      <c r="F2" s="213" t="s">
+      <c r="F2" s="227" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="214"/>
-      <c r="H2" s="214"/>
-      <c r="I2" s="214"/>
-      <c r="J2" s="215"/>
+      <c r="G2" s="228"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="228"/>
+      <c r="J2" s="229"/>
       <c r="K2" s="45"/>
-      <c r="L2" s="231"/>
-      <c r="M2" s="232"/>
-      <c r="N2" s="233"/>
+      <c r="L2" s="245"/>
+      <c r="M2" s="246"/>
+      <c r="N2" s="247"/>
     </row>
     <row r="3" spans="1:15" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="224"/>
-      <c r="B3" s="224"/>
-      <c r="C3" s="224"/>
-      <c r="D3" s="225"/>
+      <c r="A3" s="238"/>
+      <c r="B3" s="238"/>
+      <c r="C3" s="238"/>
+      <c r="D3" s="239"/>
       <c r="E3" s="33"/>
-      <c r="F3" s="216"/>
-      <c r="G3" s="217"/>
-      <c r="H3" s="217"/>
-      <c r="I3" s="217"/>
-      <c r="J3" s="218"/>
+      <c r="F3" s="230"/>
+      <c r="G3" s="231"/>
+      <c r="H3" s="231"/>
+      <c r="I3" s="231"/>
+      <c r="J3" s="232"/>
       <c r="K3" s="45"/>
-      <c r="L3" s="231"/>
-      <c r="M3" s="232"/>
-      <c r="N3" s="233"/>
+      <c r="L3" s="245"/>
+      <c r="M3" s="246"/>
+      <c r="N3" s="247"/>
     </row>
     <row r="4" spans="1:15" s="3" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="226"/>
-      <c r="B4" s="226"/>
-      <c r="C4" s="226"/>
-      <c r="D4" s="227"/>
+      <c r="A4" s="240"/>
+      <c r="B4" s="240"/>
+      <c r="C4" s="240"/>
+      <c r="D4" s="241"/>
       <c r="E4" s="33"/>
-      <c r="F4" s="219"/>
-      <c r="G4" s="220"/>
-      <c r="H4" s="220"/>
-      <c r="I4" s="220"/>
-      <c r="J4" s="221"/>
+      <c r="F4" s="233"/>
+      <c r="G4" s="234"/>
+      <c r="H4" s="234"/>
+      <c r="I4" s="234"/>
+      <c r="J4" s="235"/>
       <c r="K4" s="45"/>
-      <c r="L4" s="234"/>
-      <c r="M4" s="235"/>
-      <c r="N4" s="236"/>
+      <c r="L4" s="248"/>
+      <c r="M4" s="249"/>
+      <c r="N4" s="250"/>
     </row>
     <row r="5" spans="1:15" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
@@ -4476,11 +4476,11 @@
         <v>376</v>
       </c>
       <c r="K7" s="45"/>
-      <c r="L7" s="237" t="s">
+      <c r="L7" s="251" t="s">
         <v>185</v>
       </c>
-      <c r="M7" s="238"/>
-      <c r="N7" s="239"/>
+      <c r="M7" s="252"/>
+      <c r="N7" s="253"/>
       <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -4699,7 +4699,7 @@
         <v>380</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="250" t="s">
+      <c r="H13" s="216" t="s">
         <v>256</v>
       </c>
       <c r="I13" s="6" t="s">
@@ -4775,7 +4775,7 @@
         <v>382</v>
       </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="256" t="s">
+      <c r="H15" s="222" t="s">
         <v>432</v>
       </c>
       <c r="I15" s="6" t="s">
@@ -4813,7 +4813,7 @@
         <v>383</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="249">
+      <c r="H16" s="215">
         <v>1</v>
       </c>
       <c r="I16" s="6" t="s">
@@ -4969,7 +4969,7 @@
         <v>384</v>
       </c>
       <c r="G20" s="6"/>
-      <c r="H20" s="254" t="s">
+      <c r="H20" s="220" t="s">
         <v>434</v>
       </c>
       <c r="I20" s="6" t="s">
@@ -5277,7 +5277,7 @@
       <c r="G28" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="H28" s="257" t="s">
+      <c r="H28" s="223" t="s">
         <v>437</v>
       </c>
       <c r="I28" s="6" t="s">
@@ -5340,7 +5340,7 @@
         <v>387</v>
       </c>
       <c r="G30" s="6"/>
-      <c r="H30" s="255" t="s">
+      <c r="H30" s="221" t="s">
         <v>435</v>
       </c>
       <c r="I30" s="6" t="s">
@@ -6262,7 +6262,7 @@
         <v>397</v>
       </c>
       <c r="G64" s="6"/>
-      <c r="H64" s="251" t="s">
+      <c r="H64" s="217" t="s">
         <v>422</v>
       </c>
       <c r="I64" s="6" t="s">
@@ -6286,7 +6286,7 @@
         <v>98</v>
       </c>
       <c r="G65" s="6"/>
-      <c r="H65" s="248">
+      <c r="H65" s="214">
         <v>9564</v>
       </c>
       <c r="I65" s="6" t="s">
@@ -6426,11 +6426,11 @@
         <v>100</v>
       </c>
       <c r="G71" s="6"/>
-      <c r="H71" s="247" t="s">
+      <c r="H71" s="257" t="s">
         <v>208</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>9</v>
+        <v>212</v>
       </c>
       <c r="J71" s="44" t="s">
         <v>213</v>
@@ -6450,7 +6450,7 @@
         <v>399</v>
       </c>
       <c r="G72" s="6"/>
-      <c r="H72" s="246" t="s">
+      <c r="H72" s="213" t="s">
         <v>417</v>
       </c>
       <c r="I72" s="6" t="s">
@@ -6498,7 +6498,7 @@
         <v>401</v>
       </c>
       <c r="G74" s="6"/>
-      <c r="H74" s="245"/>
+      <c r="H74" s="212"/>
       <c r="I74" s="6" t="s">
         <v>415</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>402</v>
       </c>
       <c r="G75" s="6"/>
-      <c r="H75" s="244"/>
+      <c r="H75" s="211"/>
       <c r="I75" s="6" t="s">
         <v>414</v>
       </c>
@@ -6617,7 +6617,7 @@
         <v>103</v>
       </c>
       <c r="G81" s="6"/>
-      <c r="H81" s="253" t="s">
+      <c r="H81" s="219" t="s">
         <v>285</v>
       </c>
       <c r="I81" s="6" t="s">
@@ -6632,7 +6632,7 @@
         <v>400</v>
       </c>
       <c r="G82" s="6"/>
-      <c r="H82" s="252" t="s">
+      <c r="H82" s="218" t="s">
         <v>427</v>
       </c>
       <c r="I82" s="6" t="s">
@@ -6734,7 +6734,7 @@
       <c r="F91" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="G91" s="243" t="s">
+      <c r="G91" s="210" t="s">
         <v>407</v>
       </c>
       <c r="H91" s="173"/>
@@ -6756,7 +6756,7 @@
       <c r="F93" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="G93" s="243" t="s">
+      <c r="G93" s="210" t="s">
         <v>410</v>
       </c>
       <c r="H93" s="173"/>
@@ -6822,7 +6822,7 @@
       <c r="F99" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G99" s="243" t="s">
+      <c r="G99" s="210" t="s">
         <v>412</v>
       </c>
       <c r="H99" s="209"/>

</xml_diff>

<commit_message>
Change new lines since open indicator color
</commit_message>
<xml_diff>
--- a/Making Text Pretty - Syntax Coloring and Color Palettes/Color Palettes/MishMash-EPP-Worksheet.xlsx
+++ b/Making Text Pretty - Syntax Coloring and Color Palettes/Color Palettes/MishMash-EPP-Worksheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="440">
   <si>
     <t>Name in JGSoft Custom Syntax Coloring Scheme</t>
   </si>
@@ -2746,7 +2746,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2946,6 +2946,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF214283"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF606366"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3157,7 +3163,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="258">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3750,6 +3756,9 @@
     <xf numFmtId="0" fontId="112" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3849,7 +3858,7 @@
     <xf numFmtId="0" fontId="24" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3862,6 +3871,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF606366"/>
       <color rgb="FFA9B7C6"/>
       <color rgb="FF32593D"/>
       <color rgb="FFBFBFBF"/>
@@ -3871,7 +3881,6 @@
       <color rgb="FF555555"/>
       <color rgb="FFAE8ABE"/>
       <color rgb="FF313335"/>
-      <color rgb="FF606366"/>
     </mruColors>
   </colors>
   <extLst>
@@ -4282,7 +4291,7 @@
   <dimension ref="A1:O104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D55" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4304,76 +4313,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="254" t="s">
+      <c r="A1" s="255" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="255"/>
-      <c r="C1" s="255"/>
-      <c r="D1" s="256"/>
+      <c r="B1" s="256"/>
+      <c r="C1" s="256"/>
+      <c r="D1" s="257"/>
       <c r="E1" s="35"/>
-      <c r="F1" s="224" t="s">
+      <c r="F1" s="225" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="225"/>
-      <c r="H1" s="225"/>
-      <c r="I1" s="225"/>
-      <c r="J1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="226"/>
+      <c r="I1" s="226"/>
+      <c r="J1" s="227"/>
       <c r="K1" s="45"/>
-      <c r="L1" s="242" t="s">
+      <c r="L1" s="243" t="s">
         <v>229</v>
       </c>
-      <c r="M1" s="243"/>
-      <c r="N1" s="244"/>
+      <c r="M1" s="244"/>
+      <c r="N1" s="245"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="236"/>
-      <c r="B2" s="236"/>
-      <c r="C2" s="236"/>
-      <c r="D2" s="237"/>
+      <c r="A2" s="237"/>
+      <c r="B2" s="237"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="238"/>
       <c r="E2" s="32"/>
-      <c r="F2" s="227" t="s">
+      <c r="F2" s="228" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="229"/>
+      <c r="G2" s="229"/>
+      <c r="H2" s="229"/>
+      <c r="I2" s="229"/>
+      <c r="J2" s="230"/>
       <c r="K2" s="45"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="246"/>
-      <c r="N2" s="247"/>
+      <c r="L2" s="246"/>
+      <c r="M2" s="247"/>
+      <c r="N2" s="248"/>
     </row>
     <row r="3" spans="1:15" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="238"/>
-      <c r="B3" s="238"/>
-      <c r="C3" s="238"/>
-      <c r="D3" s="239"/>
+      <c r="A3" s="239"/>
+      <c r="B3" s="239"/>
+      <c r="C3" s="239"/>
+      <c r="D3" s="240"/>
       <c r="E3" s="33"/>
-      <c r="F3" s="230"/>
-      <c r="G3" s="231"/>
-      <c r="H3" s="231"/>
-      <c r="I3" s="231"/>
-      <c r="J3" s="232"/>
+      <c r="F3" s="231"/>
+      <c r="G3" s="232"/>
+      <c r="H3" s="232"/>
+      <c r="I3" s="232"/>
+      <c r="J3" s="233"/>
       <c r="K3" s="45"/>
-      <c r="L3" s="245"/>
-      <c r="M3" s="246"/>
-      <c r="N3" s="247"/>
+      <c r="L3" s="246"/>
+      <c r="M3" s="247"/>
+      <c r="N3" s="248"/>
     </row>
     <row r="4" spans="1:15" s="3" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="240"/>
-      <c r="B4" s="240"/>
-      <c r="C4" s="240"/>
-      <c r="D4" s="241"/>
+      <c r="A4" s="241"/>
+      <c r="B4" s="241"/>
+      <c r="C4" s="241"/>
+      <c r="D4" s="242"/>
       <c r="E4" s="33"/>
-      <c r="F4" s="233"/>
-      <c r="G4" s="234"/>
-      <c r="H4" s="234"/>
-      <c r="I4" s="234"/>
-      <c r="J4" s="235"/>
+      <c r="F4" s="234"/>
+      <c r="G4" s="235"/>
+      <c r="H4" s="235"/>
+      <c r="I4" s="235"/>
+      <c r="J4" s="236"/>
       <c r="K4" s="45"/>
-      <c r="L4" s="248"/>
-      <c r="M4" s="249"/>
-      <c r="N4" s="250"/>
+      <c r="L4" s="249"/>
+      <c r="M4" s="250"/>
+      <c r="N4" s="251"/>
     </row>
     <row r="5" spans="1:15" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
@@ -4476,11 +4485,11 @@
         <v>376</v>
       </c>
       <c r="K7" s="45"/>
-      <c r="L7" s="251" t="s">
+      <c r="L7" s="252" t="s">
         <v>185</v>
       </c>
-      <c r="M7" s="252"/>
-      <c r="N7" s="253"/>
+      <c r="M7" s="253"/>
+      <c r="N7" s="254"/>
       <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -6426,7 +6435,7 @@
         <v>100</v>
       </c>
       <c r="G71" s="6"/>
-      <c r="H71" s="257" t="s">
+      <c r="H71" s="224" t="s">
         <v>208</v>
       </c>
       <c r="I71" s="6" t="s">
@@ -6518,11 +6527,13 @@
         <v>402</v>
       </c>
       <c r="G75" s="6"/>
-      <c r="H75" s="211"/>
+      <c r="H75" s="258"/>
       <c r="I75" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="J75" s="211" t="s">
         <v>414</v>
       </c>
-      <c r="J75" s="6"/>
       <c r="K75" s="45"/>
       <c r="L75" s="50"/>
       <c r="M75" s="6"/>

</xml_diff>

<commit_message>
Update green comment and embedded link colors
</commit_message>
<xml_diff>
--- a/Making Text Pretty - Syntax Coloring and Color Palettes/Color Palettes/MishMash-EPP-Worksheet.xlsx
+++ b/Making Text Pretty - Syntax Coloring and Color Palettes/Color Palettes/MishMash-EPP-Worksheet.xlsx
@@ -1886,7 +1886,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="113" x14ac:knownFonts="1">
+  <fonts count="114" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2731,7 +2731,15 @@
     </font>
     <font>
       <b/>
-      <u/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFCBD1D1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="12"/>
       <color rgb="FF7F9F7F"/>
       <name val="Consolas"/>
@@ -2739,9 +2747,9 @@
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FFCBD1D1"/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF629755"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -3163,7 +3171,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="259">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3751,12 +3759,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="111" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="112" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3858,7 +3866,10 @@
     <xf numFmtId="0" fontId="24" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="112" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3871,6 +3882,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF7F9F7F"/>
+      <color rgb="FF629755"/>
       <color rgb="FF606366"/>
       <color rgb="FFA9B7C6"/>
       <color rgb="FF32593D"/>
@@ -3879,8 +3892,6 @@
       <color rgb="FFB5B5B5"/>
       <color rgb="FFB56277"/>
       <color rgb="FF555555"/>
-      <color rgb="FFAE8ABE"/>
-      <color rgb="FF313335"/>
     </mruColors>
   </colors>
   <extLst>
@@ -4290,8 +4301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D55" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView tabSelected="1" topLeftCell="F34" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4784,11 +4795,11 @@
         <v>382</v>
       </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="222" t="s">
+      <c r="H15" s="259" t="s">
         <v>432</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>160</v>
@@ -5286,7 +5297,7 @@
       <c r="G28" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="H28" s="223" t="s">
+      <c r="H28" s="222" t="s">
         <v>437</v>
       </c>
       <c r="I28" s="6" t="s">
@@ -6085,11 +6096,11 @@
       <c r="G56" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H56" s="199" t="s">
+      <c r="H56" s="258" t="s">
         <v>280</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>160</v>
@@ -6435,7 +6446,7 @@
         <v>100</v>
       </c>
       <c r="G71" s="6"/>
-      <c r="H71" s="224" t="s">
+      <c r="H71" s="223" t="s">
         <v>208</v>
       </c>
       <c r="I71" s="6" t="s">
@@ -6527,7 +6538,7 @@
         <v>402</v>
       </c>
       <c r="G75" s="6"/>
-      <c r="H75" s="258"/>
+      <c r="H75" s="224"/>
       <c r="I75" s="6" t="s">
         <v>212</v>
       </c>

</xml_diff>